<commit_message>
Added Doctor add new appointment slot function
</commit_message>
<xml_diff>
--- a/Java Files/AppointmentOutcome.xlsx
+++ b/Java Files/AppointmentOutcome.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sad_b\OneDrive\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB9AB6F3-6E77-4E65-AAE5-37AAB02155A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{654884DD-4F4D-4978-A420-2EDA4C0BB7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="1848" windowWidth="12048" windowHeight="8880" xr2:uid="{163CF77E-6435-4A63-BA38-B3E66022D3D1}"/>
+    <workbookView xWindow="-336" yWindow="372" windowWidth="17292" windowHeight="9840" xr2:uid="{163CF77E-6435-4A63-BA38-B3E66022D3D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>AppointmentOutcomeID</t>
   </si>
@@ -51,6 +47,21 @@
   </si>
   <si>
     <t>PrescriptionStatus</t>
+  </si>
+  <si>
+    <t>AC001</t>
+  </si>
+  <si>
+    <t>A001</t>
+  </si>
+  <si>
+    <t>MR3c45380b</t>
+  </si>
+  <si>
+    <t>Diagnosis done</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -422,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C961F069-447C-468A-928B-C5014B42E68E}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,6 +458,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>